<commit_message>
Average test excel newWatcher maven
</commit_message>
<xml_diff>
--- a/src/test/resources/average1.xlsx
+++ b/src/test/resources/average1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olegh\git\ahoo-avarage\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olegh\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A31CB4-DE75-4BF7-A911-3665AAE8119B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629223D5-1159-4135-8DF6-D486404158E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29235" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2740" yWindow="1390" windowWidth="14400" windowHeight="7590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -340,12 +340,12 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>2</v>
       </c>
@@ -356,7 +356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -373,7 +373,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -387,7 +387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -398,7 +398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -415,7 +415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -429,18 +429,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>